<commit_message>
update Demo.py, Figures.py and add new figures
</commit_message>
<xml_diff>
--- a/code/Python/Figures_WP1/WP1_Table_2_sub-all_ses-both.xlsx
+++ b/code/Python/Figures_WP1/WP1_Table_2_sub-all_ses-both.xlsx
@@ -492,19 +492,19 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>-210.149</v>
+        <v>-156.374</v>
       </c>
       <c r="E2" t="n">
-        <v>-2.033</v>
+        <v>-1.848</v>
       </c>
       <c r="F2" t="n">
-        <v>0.042</v>
+        <v>0.065</v>
       </c>
       <c r="G2" t="n">
-        <v>-412.778</v>
+        <v>-322.229</v>
       </c>
       <c r="H2" t="n">
-        <v>-7.52</v>
+        <v>9.481999999999999</v>
       </c>
     </row>
     <row r="3">
@@ -516,19 +516,19 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>-162.459</v>
+        <v>-118.148</v>
       </c>
       <c r="E3" t="n">
-        <v>-7.137</v>
+        <v>-6.341</v>
       </c>
       <c r="F3" t="n">
         <v>0</v>
       </c>
       <c r="G3" t="n">
-        <v>-207.077</v>
+        <v>-154.666</v>
       </c>
       <c r="H3" t="n">
-        <v>-117.842</v>
+        <v>-81.63</v>
       </c>
     </row>
     <row r="4">
@@ -540,19 +540,19 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>-95.71599999999999</v>
+        <v>-69.48</v>
       </c>
       <c r="E4" t="n">
-        <v>-4.205</v>
+        <v>-3.728</v>
       </c>
       <c r="F4" t="n">
         <v>0</v>
       </c>
       <c r="G4" t="n">
-        <v>-140.334</v>
+        <v>-106.008</v>
       </c>
       <c r="H4" t="n">
-        <v>-51.099</v>
+        <v>-32.953</v>
       </c>
     </row>
     <row r="5">
@@ -572,19 +572,19 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>1.728</v>
+        <v>-3.458</v>
       </c>
       <c r="E5" t="n">
-        <v>0.348</v>
+        <v>-0.68</v>
       </c>
       <c r="F5" t="n">
-        <v>0.728</v>
+        <v>0.497</v>
       </c>
       <c r="G5" t="n">
-        <v>-8.016</v>
+        <v>-13.426</v>
       </c>
       <c r="H5" t="n">
-        <v>11.472</v>
+        <v>6.51</v>
       </c>
     </row>
     <row r="6">
@@ -596,19 +596,19 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>9.881</v>
+        <v>7.267</v>
       </c>
       <c r="E6" t="n">
-        <v>9.026999999999999</v>
+        <v>6.489</v>
       </c>
       <c r="F6" t="n">
         <v>0</v>
       </c>
       <c r="G6" t="n">
-        <v>7.736</v>
+        <v>5.072</v>
       </c>
       <c r="H6" t="n">
-        <v>12.027</v>
+        <v>9.461</v>
       </c>
     </row>
     <row r="7">
@@ -620,19 +620,19 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>9.635</v>
+        <v>8.551</v>
       </c>
       <c r="E7" t="n">
-        <v>8.801</v>
+        <v>7.634</v>
       </c>
       <c r="F7" t="n">
         <v>0</v>
       </c>
       <c r="G7" t="n">
-        <v>7.489</v>
+        <v>6.355</v>
       </c>
       <c r="H7" t="n">
-        <v>11.78</v>
+        <v>10.746</v>
       </c>
     </row>
     <row r="8">
@@ -652,19 +652,19 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>55.991</v>
+        <v>26.43</v>
       </c>
       <c r="E8" t="n">
-        <v>3.337</v>
+        <v>4.805</v>
       </c>
       <c r="F8" t="n">
-        <v>0.001</v>
+        <v>0</v>
       </c>
       <c r="G8" t="n">
-        <v>23.102</v>
+        <v>15.65</v>
       </c>
       <c r="H8" t="n">
-        <v>88.881</v>
+        <v>37.211</v>
       </c>
     </row>
     <row r="9">
@@ -676,19 +676,19 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>-12.864</v>
+        <v>-5.798</v>
       </c>
       <c r="E9" t="n">
-        <v>-3.505</v>
+        <v>-4.321</v>
       </c>
       <c r="F9" t="n">
         <v>0</v>
       </c>
       <c r="G9" t="n">
-        <v>-20.057</v>
+        <v>-8.428000000000001</v>
       </c>
       <c r="H9" t="n">
-        <v>-5.671</v>
+        <v>-3.168</v>
       </c>
     </row>
     <row r="10">
@@ -700,19 +700,19 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>-25.504</v>
+        <v>-11.218</v>
       </c>
       <c r="E10" t="n">
-        <v>-6.72</v>
+        <v>-8.791</v>
       </c>
       <c r="F10" t="n">
         <v>0</v>
       </c>
       <c r="G10" t="n">
-        <v>-32.942</v>
+        <v>-13.719</v>
       </c>
       <c r="H10" t="n">
-        <v>-18.066</v>
+        <v>-8.717000000000001</v>
       </c>
     </row>
     <row r="11">
@@ -732,19 +732,19 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>-7.638</v>
+        <v>-3.87</v>
       </c>
       <c r="E11" t="n">
-        <v>-0.896</v>
+        <v>-0.54</v>
       </c>
       <c r="F11" t="n">
-        <v>0.37</v>
+        <v>0.589</v>
       </c>
       <c r="G11" t="n">
-        <v>-24.353</v>
+        <v>-17.916</v>
       </c>
       <c r="H11" t="n">
-        <v>9.077</v>
+        <v>10.176</v>
       </c>
     </row>
     <row r="12">
@@ -756,19 +756,19 @@
         </is>
       </c>
       <c r="D12" t="n">
-        <v>11.685</v>
+        <v>11.44</v>
       </c>
       <c r="E12" t="n">
-        <v>6.264</v>
+        <v>6.58</v>
       </c>
       <c r="F12" t="n">
         <v>0</v>
       </c>
       <c r="G12" t="n">
-        <v>8.029</v>
+        <v>8.032</v>
       </c>
       <c r="H12" t="n">
-        <v>15.341</v>
+        <v>14.848</v>
       </c>
     </row>
     <row r="13">
@@ -780,19 +780,19 @@
         </is>
       </c>
       <c r="D13" t="n">
-        <v>16.534</v>
+        <v>13.388</v>
       </c>
       <c r="E13" t="n">
-        <v>8.574</v>
+        <v>8.083</v>
       </c>
       <c r="F13" t="n">
         <v>0</v>
       </c>
       <c r="G13" t="n">
-        <v>12.754</v>
+        <v>10.142</v>
       </c>
       <c r="H13" t="n">
-        <v>20.313</v>
+        <v>16.634</v>
       </c>
     </row>
   </sheetData>

</xml_diff>